<commit_message>
Handle inproper input and added examples to documentation.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\Desktop\Dissertation app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\PycharmProjects\dissertation-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87627E8-A8E8-4F9A-9538-03FF14560D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E233A6-6146-49FF-9DDE-C1089A999F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="1485" windowWidth="21600" windowHeight="11385" tabRatio="684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="1485" windowWidth="21600" windowHeight="11385" tabRatio="684" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cattle" sheetId="12" r:id="rId1"/>
@@ -1097,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85C816C-F2F8-4069-80D5-E3DF17509B0E}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -9297,13 +9297,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEAA06E-F330-4153-A681-769C8DA29C30}">
   <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView topLeftCell="J10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P23" sqref="P23:AK39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added function for just signs and ids
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\PycharmProjects\dissertation-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1774A4D-48CB-424C-B4B6-890915FC037A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF7DEF3-DEAA-43D7-A4B4-C9F72373235B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30135" yWindow="1290" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cattle" sheetId="12" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="201">
   <si>
     <t>Diarrhoea</t>
   </si>
@@ -397,9 +397,6 @@
   </si>
   <si>
     <t>Ascaris_foals</t>
-  </si>
-  <si>
-    <t>Babisiosis</t>
   </si>
   <si>
     <t>GI_non-infectious_colic</t>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17">
         <v>0.79379999999999995</v>
@@ -2184,7 +2181,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2192,10 +2189,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2206,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2214,10 +2211,10 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2225,10 +2222,10 @@
         <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2239,7 +2236,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2250,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2261,7 +2258,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2272,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2280,10 +2277,10 @@
         <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2294,7 +2291,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,7 +2302,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,7 +2313,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2327,7 +2324,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2335,10 +2332,10 @@
         <v>57</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2346,10 +2343,10 @@
         <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2371,7 +2368,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2399,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,10 +2407,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2424,7 +2421,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2432,10 +2429,10 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2443,10 +2440,10 @@
         <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2457,7 +2454,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2468,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2479,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2490,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2498,10 +2495,10 @@
         <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2512,7 +2509,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2523,7 +2520,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2534,7 +2531,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2545,7 +2542,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,10 +2550,10 @@
         <v>57</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2564,10 +2561,10 @@
         <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2578,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2589,7 +2586,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2620,7 +2617,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2631,7 +2628,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2639,10 +2636,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2653,7 +2650,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2664,7 +2661,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2675,7 +2672,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2697,7 +2694,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2708,7 +2705,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2719,7 +2716,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2730,7 +2727,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2741,7 +2738,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2752,7 +2749,7 @@
         <v>74</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2760,10 +2757,10 @@
         <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2774,7 +2771,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2785,7 +2782,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2793,10 +2790,10 @@
         <v>57</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2807,7 +2804,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2818,7 +2815,7 @@
         <v>76</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2840,7 +2837,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2853,7 +2850,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,10 +2865,10 @@
         <v>91</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2882,7 +2879,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2890,10 +2887,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2901,10 +2898,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2915,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2923,10 +2920,10 @@
         <v>93</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2934,10 +2931,10 @@
         <v>94</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2948,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2956,10 +2953,10 @@
         <v>95</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2970,7 +2967,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2981,7 +2978,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2989,10 +2986,10 @@
         <v>96</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3000,21 +2997,21 @@
         <v>97</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3025,7 +3022,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3036,7 +3033,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3047,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3058,7 +3055,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3086,10 +3083,10 @@
         <v>91</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3100,7 +3097,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3108,10 +3105,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3119,10 +3116,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3133,7 +3130,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3141,10 +3138,10 @@
         <v>93</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3152,10 +3149,10 @@
         <v>94</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3166,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3174,10 +3171,10 @@
         <v>95</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3188,7 +3185,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3199,7 +3196,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3207,10 +3204,10 @@
         <v>96</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3218,21 +3215,21 @@
         <v>97</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,7 +3240,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3254,7 +3251,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3265,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3276,7 +3273,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3288,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B79A8A-1D7B-4FD1-8C3C-2C5F3A1811C5}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3303,7 +3300,7 @@
         <v>98</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3311,7 +3308,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3319,7 +3316,7 @@
         <v>99</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3327,7 +3324,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3335,7 +3332,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3343,7 +3340,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3351,7 +3348,7 @@
         <v>77</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3359,7 +3356,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3367,7 +3364,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3375,7 +3372,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3383,7 +3380,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3391,7 +3388,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3399,7 +3396,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3407,7 +3404,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3415,31 +3412,31 @@
         <v>20</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3447,15 +3444,15 @@
         <v>33</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3463,7 +3460,7 @@
         <v>78</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3471,7 +3468,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3479,7 +3476,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3487,31 +3484,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3519,7 +3516,7 @@
         <v>35</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3527,7 +3524,7 @@
         <v>36</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3535,7 +3532,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3543,7 +3540,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3551,7 +3548,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32" s="7"/>
     </row>
@@ -3560,7 +3557,7 @@
         <v>80</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3568,7 +3565,7 @@
         <v>40</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3576,7 +3573,7 @@
         <v>38</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3584,7 +3581,7 @@
         <v>81</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3592,39 +3589,39 @@
         <v>26</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3632,7 +3629,7 @@
         <v>82</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3640,23 +3637,23 @@
         <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3664,7 +3661,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3672,7 +3669,7 @@
         <v>27</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3680,7 +3677,7 @@
         <v>28</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -7495,7 +7492,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8726,7 +8723,7 @@
         <v>97</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>55</v>
@@ -8920,7 +8917,7 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B5" s="15">
         <v>5.6250000000000001E-2</v>
@@ -8979,7 +8976,7 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="15">
         <v>0.91249999999999998</v>
@@ -9038,7 +9035,7 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="15">
         <v>0.58750000000000002</v>
@@ -9097,7 +9094,7 @@
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="15">
         <v>5.6250000000000001E-2</v>
@@ -9156,7 +9153,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="15">
         <v>5.6250000000000001E-2</v>
@@ -9215,7 +9212,7 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9274,7 +9271,7 @@
     </row>
     <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9333,7 +9330,7 @@
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9451,7 +9448,7 @@
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9510,7 +9507,7 @@
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9569,7 +9566,7 @@
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9628,7 +9625,7 @@
     </row>
     <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9687,7 +9684,7 @@
     </row>
     <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="15">
         <v>2.5000000000000001E-2</v>
@@ -9746,7 +9743,7 @@
     </row>
     <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19" s="15">
         <v>5.6250000000000001E-2</v>
@@ -9985,7 +9982,7 @@
         <v>97</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>55</v>
@@ -10120,7 +10117,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B4" s="9">
         <v>6.6666666666666666E-2</v>
@@ -10179,7 +10176,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="9">
         <v>0.61875000000000002</v>
@@ -10238,7 +10235,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="9">
         <v>0.5</v>
@@ -10297,7 +10294,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="9">
         <v>5.6250000000000001E-2</v>
@@ -10356,7 +10353,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10415,7 +10412,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10533,7 +10530,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10592,7 +10589,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10651,7 +10648,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10710,7 +10707,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10769,7 +10766,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="9">
         <v>2.5000000000000001E-2</v>
@@ -10828,7 +10825,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="9">
         <v>5.6250000000000001E-2</v>
@@ -11013,8 +11010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEAA06E-F330-4153-A681-769C8DA29C30}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C34" sqref="A34:C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11032,7 +11029,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -11040,10 +11037,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -11054,7 +11051,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -11062,10 +11059,10 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -11076,7 +11073,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -11087,7 +11084,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -11098,7 +11095,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -11106,10 +11103,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -11120,7 +11117,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -11131,7 +11128,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -11142,7 +11139,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -11150,10 +11147,10 @@
         <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -11161,10 +11158,10 @@
         <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -11175,7 +11172,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -11186,7 +11183,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -11194,10 +11191,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -11208,7 +11205,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -11219,7 +11216,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -11230,7 +11227,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -11241,7 +11238,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -11252,7 +11249,7 @@
         <v>73</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -11263,7 +11260,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -11274,7 +11271,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -11285,7 +11282,7 @@
         <v>74</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -11296,7 +11293,7 @@
         <v>75</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -11307,7 +11304,7 @@
         <v>76</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11315,10 +11312,10 @@
         <v>91</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11326,10 +11323,10 @@
         <v>92</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11337,10 +11334,10 @@
         <v>93</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11348,10 +11345,10 @@
         <v>94</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11359,10 +11356,10 @@
         <v>95</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11370,10 +11367,10 @@
         <v>96</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -11381,21 +11378,21 @@
         <v>97</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -11437,7 +11434,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -11445,10 +11442,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -11459,7 +11456,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -11467,10 +11464,10 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -11481,7 +11478,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -11492,7 +11489,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -11503,7 +11500,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -11511,10 +11508,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -11525,7 +11522,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -11536,7 +11533,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -11547,7 +11544,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -11555,10 +11552,10 @@
         <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -11566,10 +11563,10 @@
         <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -11580,7 +11577,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -11591,7 +11588,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed when workbook is loaded to hopefully improve performance
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\PycharmProjects\dissertation-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF7DEF3-DEAA-43D7-A4B4-C9F72373235B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB8E930-7EAA-47EE-ABCB-56290C8DCF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30135" yWindow="1290" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cattle" sheetId="12" r:id="rId1"/>
@@ -2162,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5241CE2-746E-4D41-B8AB-B98FD964D1A9}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,7 +3286,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,7 +3696,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11010,8 +11010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEAA06E-F330-4153-A681-769C8DA29C30}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
actually fixed loading of workbook, perfomance should improve significantly
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\PycharmProjects\dissertation-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB8E930-7EAA-47EE-ABCB-56290C8DCF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E6676-303D-46D4-A7B0-5C568A04F63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cattle" sheetId="12" r:id="rId1"/>
@@ -2162,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5241CE2-746E-4D41-B8AB-B98FD964D1A9}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B79A8A-1D7B-4FD1-8C3C-2C5F3A1811C5}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>178</v>
@@ -3696,7 +3696,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B7" s="10">
         <v>2.5000000000000001E-2</v>
@@ -4602,7 +4602,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>2.5000000000000001E-2</v>

</xml_diff>

<commit_message>
Fixed error messages further so they include what is causing the issue
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\PycharmProjects\dissertation-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E6676-303D-46D4-A7B0-5C568A04F63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EC2445-4921-4707-86C8-04C1CAAC3A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cattle" sheetId="12" r:id="rId1"/>
     <sheet name="Sheep" sheetId="5" r:id="rId2"/>
     <sheet name="Goat" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheep vs Goat" sheetId="7" state="hidden" r:id="rId4"/>
+    <sheet name="Sheep vs Goat" sheetId="7" r:id="rId4"/>
     <sheet name="Camel" sheetId="14" r:id="rId5"/>
     <sheet name="Horse" sheetId="13" r:id="rId6"/>
     <sheet name="Donkey" sheetId="10" r:id="rId7"/>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,7 +3285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B79A8A-1D7B-4FD1-8C3C-2C5F3A1811C5}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -5445,10 +5445,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7476,6 +7476,57 @@
       <c r="A39" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V28">

</xml_diff>

<commit_message>
added including own matrix to achieve goal
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demkn\PycharmProjects\dissertation-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B481939C-D02C-4AB1-9AA5-FBD752BC6195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3936D4-FE78-4F61-8DC0-FBD0C94CFC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1305" windowWidth="23805" windowHeight="14175" tabRatio="684" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29790" yWindow="1185" windowWidth="23805" windowHeight="14175" tabRatio="684" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cattle" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="188">
   <si>
     <t>Diarrhoea</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Lymph Node enlargement</t>
-  </si>
-  <si>
-    <t>zz_Other</t>
   </si>
   <si>
     <t>Anae</t>
@@ -1223,49 +1220,49 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
         <v>54</v>
       </c>
-      <c r="N1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>55</v>
-      </c>
-      <c r="P1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2020,7 +2017,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>0.79379999999999995</v>
@@ -2093,200 +2090,200 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2311,233 +2308,233 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2562,200 +2559,200 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2780,200 +2777,200 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2985,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B79A8A-1D7B-4FD1-8C3C-2C5F3A1811C5}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,10 +2994,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,15 +3005,15 @@
         <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3029,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,15 +3037,15 @@
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3053,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3061,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3069,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3077,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3085,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3093,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3101,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,31 +3109,31 @@
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3144,31 +3141,31 @@
         <v>31</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3176,7 +3173,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3184,31 +3181,31 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3216,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3224,7 +3221,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3232,7 +3229,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3240,7 +3237,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3248,16 +3245,16 @@
         <v>24</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3265,7 +3262,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3273,15 +3270,15 @@
         <v>35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3289,47 +3286,47 @@
         <v>25</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3337,23 +3334,23 @@
         <v>38</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3361,7 +3358,7 @@
         <v>36</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3369,7 +3366,7 @@
         <v>26</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3377,7 +3374,7 @@
         <v>27</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3396,7 +3393,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,58 +3408,58 @@
         <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="I1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3762,7 +3759,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="10">
         <v>2.5000000000000001E-2</v>
@@ -4234,7 +4231,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B15" s="10">
         <v>0.92500000000000004</v>
@@ -4302,7 +4299,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4316,58 +4313,58 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4608,7 +4605,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>2.5000000000000001E-2</v>
@@ -5080,7 +5077,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B14">
         <v>0.91249999999999998</v>
@@ -5148,7 +5145,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5163,67 +5160,67 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -5364,7 +5361,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>2.5000000000000001E-2</v>
@@ -5500,7 +5497,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>0.36249999999999999</v>
@@ -5568,7 +5565,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>0.05</v>
@@ -5840,7 +5837,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>0.47499999999999998</v>
@@ -5976,7 +5973,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>2.5000000000000001E-2</v>
@@ -6044,7 +6041,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14">
         <v>7.4999999999999997E-2</v>
@@ -6248,7 +6245,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>0.85416666666666674</v>
@@ -6325,7 +6322,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6340,63 +6337,63 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="11">
         <v>0.14374999999999999</v>
@@ -6514,7 +6511,7 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="11">
         <v>0.67500000000000004</v>
@@ -6632,7 +6629,7 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="11">
         <v>0.91249999999999998</v>
@@ -6691,7 +6688,7 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="11">
         <v>0.58750000000000002</v>
@@ -6750,7 +6747,7 @@
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="11">
         <v>5.6250000000000001E-2</v>
@@ -6809,7 +6806,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="11">
         <v>5.6250000000000001E-2</v>
@@ -6868,7 +6865,7 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="11">
         <v>2.5000000000000001E-2</v>
@@ -6927,7 +6924,7 @@
     </row>
     <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="11">
         <v>2.5000000000000001E-2</v>
@@ -6986,7 +6983,7 @@
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7104,7 +7101,7 @@
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7163,7 +7160,7 @@
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7222,7 +7219,7 @@
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7281,7 +7278,7 @@
     </row>
     <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7340,7 +7337,7 @@
     </row>
     <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="11">
         <v>2.5000000000000001E-2</v>
@@ -7399,7 +7396,7 @@
     </row>
     <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="11">
         <v>5.6250000000000001E-2</v>
@@ -7517,7 +7514,7 @@
     </row>
     <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B21" s="11">
         <v>0.94374999999999998</v>
@@ -7584,8 +7581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7599,58 +7596,58 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -7714,7 +7711,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="9">
         <v>0.67500000000000004</v>
@@ -7832,7 +7829,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="9">
         <v>0.61875000000000002</v>
@@ -7891,7 +7888,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="9">
         <v>0.5</v>
@@ -7950,7 +7947,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="9">
         <v>5.6250000000000001E-2</v>
@@ -8009,7 +8006,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8068,7 +8065,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8186,7 +8183,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8245,7 +8242,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8304,7 +8301,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8363,7 +8360,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8422,7 +8419,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="9">
         <v>2.5000000000000001E-2</v>
@@ -8481,7 +8478,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="9">
         <v>5.6250000000000001E-2</v>
@@ -8599,7 +8596,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B18" s="9">
         <v>0.95937499999999998</v>
@@ -8679,376 +8676,376 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -9071,7 +9068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500D00D8-B9C2-4429-B601-4DF88188BD3F}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -9084,167 +9081,167 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -9269,200 +9266,200 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>